<commit_message>
Add post details via js and jquery
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/dev/lab/ajax/rails-and-ajax/ajaxblog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/dev/lab/ajax/ajaxblog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A9EE9-2BE8-C441-86A5-226722C5B2CD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07CB3F6-0F3C-9946-B02E-0B9FA65053DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14920" xr2:uid="{3ED0D812-8D90-374B-ADEB-1752FC133D99}"/>
+    <workbookView xWindow="820" yWindow="-16420" windowWidth="25600" windowHeight="14900" xr2:uid="{3ED0D812-8D90-374B-ADEB-1752FC133D99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>dataType</t>
   </si>
@@ -33,29 +33,56 @@
     <t>method</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>rails</t>
-  </si>
-  <si>
-    <t>jquery</t>
-  </si>
-  <si>
-    <t>javascript</t>
-  </si>
-  <si>
     <t>funcionality</t>
   </si>
   <si>
-    <t>rrrrrr</t>
+    <t>render a list</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>/items/:id</t>
+  </si>
+  <si>
+    <t>/items</t>
+  </si>
+  <si>
+    <t>$.get('/items')</t>
+  </si>
+  <si>
+    <t>fetch('/items')</t>
+  </si>
+  <si>
+    <t>AJAX</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>JQuery</t>
+  </si>
+  <si>
+    <t>$.GET('/items/:id')</t>
+  </si>
+  <si>
+    <t>$.ajax({})</t>
+  </si>
+  <si>
+    <t>Rails route</t>
+  </si>
+  <si>
+    <t>render item has_many</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -64,8 +91,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,11 +141,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,179 +472,207 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="21.33203125" style="2"/>
+    <col min="5" max="5" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="21.33203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update after study group
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/dev/lab/ajax/ajaxblog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07CB3F6-0F3C-9946-B02E-0B9FA65053DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31747C5-32B0-8548-8FFB-45070BA4C86B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-16420" windowWidth="25600" windowHeight="14900" xr2:uid="{3ED0D812-8D90-374B-ADEB-1752FC133D99}"/>
+    <workbookView xWindow="-14140" yWindow="-14900" windowWidth="25600" windowHeight="14900" xr2:uid="{3ED0D812-8D90-374B-ADEB-1752FC133D99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>dataType</t>
   </si>
@@ -66,9 +66,6 @@
     <t>JQuery</t>
   </si>
   <si>
-    <t>$.GET('/items/:id')</t>
-  </si>
-  <si>
     <t>$.ajax({})</t>
   </si>
   <si>
@@ -76,6 +73,21 @@
   </si>
   <si>
     <t>render item has_many</t>
+  </si>
+  <si>
+    <t>render a form</t>
+  </si>
+  <si>
+    <t>Handlebars</t>
+  </si>
+  <si>
+    <t>HTML from Rails</t>
+  </si>
+  <si>
+    <t>$.get('/items/:id')</t>
+  </si>
+  <si>
+    <t>fetch('/items/:id')</t>
   </si>
 </sst>
 </file>
@@ -469,18 +481,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EAA10F-AC34-DD4D-83B3-F114B37BAE0E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="21.33203125" style="2"/>
+    <col min="2" max="2" width="21.33203125" style="2"/>
+    <col min="3" max="3" width="24.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="2"/>
     <col min="5" max="5" width="27.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="21.33203125" style="2"/>
+    <col min="6" max="6" width="21.33203125" style="2"/>
+    <col min="7" max="7" width="26" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="21.33203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.2">
@@ -494,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>12</v>
@@ -523,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
@@ -531,7 +547,7 @@
     </row>
     <row r="3" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -543,33 +559,49 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -674,6 +706,12 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
+    <row r="18" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>